<commit_message>
Fix typos in VII yamls
</commit_message>
<xml_diff>
--- a/inc/flattened/createYaml/VII-splitstem.xlsx
+++ b/inc/flattened/createYaml/VII-splitstem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/giellalt/lang-ciw/inc/flattened/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5EBB75-34A5-064B-B4BA-F65BBD949F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1264DC-E9A1-0642-AE12-8919737E20FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27320" yWindow="5060" windowWidth="27320" windowHeight="14860" xr2:uid="{F60773C9-26C0-414F-936B-204C5C4D934C}"/>
   </bookViews>
@@ -1470,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA193F61-3C0D-9941-81CC-6F6AD6C92B40}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I227" sqref="I227"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8169,8 +8169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10602B5-8061-9841-B1CF-59F4D777D95C}">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" zoomScale="141" workbookViewId="0">
-      <selection activeCell="H117" sqref="H117"/>
+    <sheetView topLeftCell="A65" zoomScale="141" workbookViewId="0">
+      <selection activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11462,9 +11462,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11633,27 +11636,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CFA308-43F1-499A-8049-AAB3DA408682}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="56612388-9f28-4625-93a0-6879c02082d6"/>
-    <ds:schemaRef ds:uri="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11678,9 +11669,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CFA308-43F1-499A-8049-AAB3DA408682}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="56612388-9f28-4625-93a0-6879c02082d6"/>
+    <ds:schemaRef ds:uri="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding detail to notes
</commit_message>
<xml_diff>
--- a/inc/flattened/createYaml/VII-splitstem.xlsx
+++ b/inc/flattened/createYaml/VII-splitstem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/giellalt/lang-ciw/inc/flattened/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1264DC-E9A1-0642-AE12-8919737E20FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7F68A6-E87E-5440-B6BB-70AF5E86DA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27320" yWindow="5060" windowWidth="27320" windowHeight="14860" xr2:uid="{F60773C9-26C0-414F-936B-204C5C4D934C}"/>
+    <workbookView xWindow="4420" yWindow="3660" windowWidth="27320" windowHeight="14860" xr2:uid="{F60773C9-26C0-414F-936B-204C5C4D934C}"/>
   </bookViews>
   <sheets>
     <sheet name="VII_IND" sheetId="1" r:id="rId1"/>
@@ -1470,7 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA193F61-3C0D-9941-81CC-6F6AD6C92B40}">
   <dimension ref="A1:I257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
@@ -8169,7 +8169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10602B5-8061-9841-B1CF-59F4D777D95C}">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScale="141" workbookViewId="0">
+    <sheetView zoomScale="141" workbookViewId="0">
       <selection activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
@@ -11462,15 +11462,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EDA4FEBE11D32545B6C4D443ADFB229A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa29c2c3225ad03fb09b8df90fa91a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b103a3be-6c61-44b0-93c5-2b779aa38a01" xmlns:ns3="56612388-9f28-4625-93a0-6879c02082d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2c16c82533632c11d7fcceef7f9e9ea5" ns2:_="" ns3:_="">
     <xsd:import namespace="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
@@ -11635,6 +11626,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -11642,14 +11642,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CADB2AF-8FF4-4CD3-86AB-7AA08F493F37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11664,6 +11656,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A50646E-DC1C-4D16-AC23-4B244D7154EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>